<commit_message>
implemented ExcelWriter; to be fixed
</commit_message>
<xml_diff>
--- a/src/test/resources/valid/color/multipleYellowIntervalsSchedule.xlsx
+++ b/src/test/resources/valid/color/multipleYellowIntervalsSchedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexandrutodea/dev/schedule-matcher/src/test/resources/valid/color/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\X\IdeaProjects\SOJ-Team-Project\src\test\resources\valid\color\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD642180-FA47-3C46-B2FE-7A111B71CAC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE481057-48C2-487F-97BF-0FCD431FBC0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1520" yWindow="4060" windowWidth="27640" windowHeight="16940" xr2:uid="{908E9387-ABF5-9B43-AAD6-F9C58C7F893A}"/>
+    <workbookView xWindow="7965" yWindow="4365" windowWidth="21600" windowHeight="11325" xr2:uid="{908E9387-ABF5-9B43-AAD6-F9C58C7F893A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -88,7 +86,7 @@
     <t>16:00 - 17:00</t>
   </si>
   <si>
-    <t>9:00 -10:00</t>
+    <t>9:00 - 10:00</t>
   </si>
 </sst>
 </file>
@@ -474,12 +472,12 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -502,7 +500,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -514,7 +512,7 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -526,7 +524,7 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -538,7 +536,7 @@
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -550,7 +548,7 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -562,7 +560,7 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -574,7 +572,7 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -586,7 +584,7 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -598,7 +596,7 @@
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -610,7 +608,7 @@
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -622,7 +620,7 @@
       <c r="G11" s="2"/>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>15</v>
       </c>

</xml_diff>